<commit_message>
Finalizando relatório dos valores do sensor
</commit_message>
<xml_diff>
--- a/Excel_Dados_sensor.xlsx
+++ b/Excel_Dados_sensor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\Desktop\Arq Comp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b02399f3f135e69c/Documentos/SPTECH - 20231/sprint2/Documentacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A97890FF-05A2-4516-BE8D-B9D61F90722B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{A97890FF-05A2-4516-BE8D-B9D61F90722B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A182C9B9-0138-494E-BA5C-2A0613BBDB1C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CDC814B1-D003-4DDA-825C-D47DAC56574D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CDC814B1-D003-4DDA-825C-D47DAC56574D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="\ \°\C\ \-#.##"/>
+    <numFmt numFmtId="164" formatCode="\ \°\C\ \-#.##"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -156,13 +156,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -482,40 +482,39 @@
   <dimension ref="A2:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6328125" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="3" t="s">
@@ -567,37 +566,37 @@
         <f>MAX(A4:A53)</f>
         <v>-19.55</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="6">
-        <f>(A4*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="E4" s="5">
+        <f t="shared" ref="E4:E35" si="0">(A4*0.36) - 17.96</f>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F4" s="5">
         <f>MAX(E4:E53)</f>
         <v>-24.998000000000001</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <f>MIN(E4:E53)</f>
         <v>-34.1492</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>-18</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <f>MEDIAN(E4:E53)</f>
         <v>-26.052800000000001</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <f>AVERAGE(E4:E53)</f>
         <v>-27.243680000000019</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <f>QUARTILE(E4:E53,1)</f>
         <v>-28.166</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <f>QUARTILE(E4:E53,3)</f>
         <v>-25.703600000000002</v>
       </c>
@@ -609,17 +608,17 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="6">
-        <f>(A5*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1">
@@ -628,17 +627,17 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="6">
-        <f>(A6*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1">
@@ -647,17 +646,17 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="6">
-        <f>(A7*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1">
@@ -666,17 +665,17 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="6">
-        <f>(A8*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1">
@@ -685,17 +684,17 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="6">
-        <f>(A9*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1">
@@ -704,17 +703,17 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="6">
-        <f>(A10*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
+      <c r="E10" s="5">
+        <f t="shared" si="0"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1">
@@ -723,17 +722,17 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="6">
-        <f>(A11*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
+      <c r="E11" s="5">
+        <f t="shared" si="0"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1">
@@ -742,17 +741,17 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="6">
-        <f>(A12*0.36) - 17.96</f>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
         <v>-26.229199999999999</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="1">
@@ -761,17 +760,17 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="6">
-        <f>(A13*0.36) - 17.96</f>
+      <c r="E13" s="5">
+        <f t="shared" si="0"/>
         <v>-26.4056</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="1">
@@ -780,17 +779,17 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="6">
-        <f>(A14*0.36) - 17.96</f>
+      <c r="E14" s="5">
+        <f t="shared" si="0"/>
         <v>-26.229199999999999</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="1">
@@ -799,17 +798,17 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="6">
-        <f>(A15*0.36) - 17.96</f>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
         <v>-26.4056</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="1">
@@ -818,17 +817,17 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="6">
-        <f>(A16*0.36) - 17.96</f>
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
         <v>-26.229199999999999</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="1">
@@ -837,17 +836,17 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="6">
-        <f>(A17*0.36) - 17.96</f>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
         <v>-26.229199999999999</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="1">
@@ -856,17 +855,17 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="6">
-        <f>(A18*0.36) - 17.96</f>
+      <c r="E18" s="5">
+        <f t="shared" si="0"/>
         <v>-24.998000000000001</v>
       </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="1">
@@ -875,17 +874,17 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="6">
-        <f>(A19*0.36) - 17.96</f>
+      <c r="E19" s="5">
+        <f t="shared" si="0"/>
         <v>-26.229199999999999</v>
       </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="1">
@@ -894,17 +893,17 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="6">
-        <f>(A20*0.36) - 17.96</f>
+      <c r="E20" s="5">
+        <f t="shared" si="0"/>
         <v>-30.275600000000001</v>
       </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="1">
@@ -913,17 +912,17 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="6">
-        <f>(A21*0.36) - 17.96</f>
+      <c r="E21" s="5">
+        <f t="shared" si="0"/>
         <v>-33.090800000000002</v>
       </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="1">
@@ -932,17 +931,17 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="6">
-        <f>(A22*0.36) - 17.96</f>
+      <c r="E22" s="5">
+        <f t="shared" si="0"/>
         <v>-34.1492</v>
       </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="1">
@@ -951,17 +950,17 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="6">
-        <f>(A23*0.36) - 17.96</f>
+      <c r="E23" s="5">
+        <f t="shared" si="0"/>
         <v>-33.796399999999998</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="1">
@@ -970,17 +969,17 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="6">
-        <f>(A24*0.36) - 17.96</f>
+      <c r="E24" s="5">
+        <f t="shared" si="0"/>
         <v>-32.914400000000001</v>
       </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="1">
@@ -989,17 +988,17 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="6">
-        <f>(A25*0.36) - 17.96</f>
+      <c r="E25" s="5">
+        <f t="shared" si="0"/>
         <v>-32.212400000000002</v>
       </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="1">
@@ -1008,17 +1007,17 @@
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="6">
-        <f>(A26*0.36) - 17.96</f>
+      <c r="E26" s="5">
+        <f t="shared" si="0"/>
         <v>-31.506800000000002</v>
       </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="1">
@@ -1027,17 +1026,17 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="6">
-        <f>(A27*0.36) - 17.96</f>
+      <c r="E27" s="5">
+        <f t="shared" si="0"/>
         <v>-31.157599999999999</v>
       </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="1">
@@ -1046,17 +1045,17 @@
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="6">
-        <f>(A28*0.36) - 17.96</f>
+      <c r="E28" s="5">
+        <f t="shared" si="0"/>
         <v>-30.275600000000001</v>
       </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="1">
@@ -1065,17 +1064,17 @@
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="6">
-        <f>(A29*0.36) - 17.96</f>
+      <c r="E29" s="5">
+        <f t="shared" si="0"/>
         <v>-29.220800000000001</v>
       </c>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="1">
@@ -1084,17 +1083,17 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="6">
-        <f>(A30*0.36) - 17.96</f>
+      <c r="E30" s="5">
+        <f t="shared" si="0"/>
         <v>-28.868000000000002</v>
       </c>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="1">
@@ -1103,17 +1102,17 @@
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="6">
-        <f>(A31*0.36) - 17.96</f>
+      <c r="E31" s="5">
+        <f t="shared" si="0"/>
         <v>-28.518799999999999</v>
       </c>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="1">
@@ -1122,17 +1121,17 @@
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="6">
-        <f>(A32*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
+      <c r="E32" s="5">
+        <f t="shared" si="0"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="1">
@@ -1141,17 +1140,17 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="6">
-        <f>(A33*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
+      <c r="E33" s="5">
+        <f t="shared" si="0"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="1">
@@ -1160,17 +1159,17 @@
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="6">
-        <f>(A34*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
+      <c r="E34" s="5">
+        <f t="shared" si="0"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="1">
@@ -1179,17 +1178,17 @@
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="6">
-        <f>(A35*0.36) - 17.96</f>
+      <c r="E35" s="5">
+        <f t="shared" si="0"/>
         <v>-26.052800000000001</v>
       </c>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="1">
@@ -1198,17 +1197,17 @@
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="6">
-        <f>(A36*0.36) - 17.96</f>
+      <c r="E36" s="5">
+        <f t="shared" ref="E36:E53" si="1">(A36*0.36) - 17.96</f>
         <v>-25.8764</v>
       </c>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="1">
@@ -1217,17 +1216,17 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="6">
-        <f>(A37*0.36) - 17.96</f>
+      <c r="E37" s="5">
+        <f t="shared" si="1"/>
         <v>-26.052800000000001</v>
       </c>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="1">
@@ -1236,17 +1235,17 @@
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="6">
-        <f>(A38*0.36) - 17.96</f>
+      <c r="E38" s="5">
+        <f t="shared" si="1"/>
         <v>-26.4056</v>
       </c>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="2">
@@ -1255,17 +1254,17 @@
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="6">
-        <f>(A39*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
+      <c r="E39" s="5">
+        <f t="shared" si="1"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="2">
@@ -1274,17 +1273,17 @@
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="6">
-        <f>(A40*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
+      <c r="E40" s="5">
+        <f t="shared" si="1"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="2">
@@ -1293,17 +1292,17 @@
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="6">
-        <f>(A41*0.36) - 17.96</f>
+      <c r="E41" s="5">
+        <f t="shared" si="1"/>
         <v>-25.527200000000001</v>
       </c>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="2">
@@ -1312,17 +1311,17 @@
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="6">
-        <f>(A42*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
+      <c r="E42" s="5">
+        <f t="shared" si="1"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="2">
@@ -1331,17 +1330,17 @@
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="6">
-        <f>(A43*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
+      <c r="E43" s="5">
+        <f t="shared" si="1"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="2">
@@ -1350,17 +1349,17 @@
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
-      <c r="E44" s="6">
-        <f>(A44*0.36) - 17.96</f>
+      <c r="E44" s="5">
+        <f t="shared" si="1"/>
         <v>-25.174399999999999</v>
       </c>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="2">
@@ -1369,17 +1368,17 @@
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
-      <c r="E45" s="6">
-        <f>(A45*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
+      <c r="E45" s="5">
+        <f t="shared" si="1"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="2">
@@ -1388,17 +1387,17 @@
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
-      <c r="E46" s="6">
-        <f>(A46*0.36) - 17.96</f>
+      <c r="E46" s="5">
+        <f t="shared" si="1"/>
         <v>-25.174399999999999</v>
       </c>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="2">
@@ -1407,17 +1406,17 @@
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
-      <c r="E47" s="6">
-        <f>(A47*0.36) - 17.96</f>
+      <c r="E47" s="5">
+        <f t="shared" si="1"/>
         <v>-28.166</v>
       </c>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="1">
@@ -1426,17 +1425,17 @@
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="6">
-        <f>(A48*0.36) - 17.96</f>
+      <c r="E48" s="5">
+        <f t="shared" si="1"/>
         <v>-26.229199999999999</v>
       </c>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="1">
@@ -1445,17 +1444,17 @@
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
-      <c r="E49" s="6">
-        <f>(A49*0.36) - 17.96</f>
+      <c r="E49" s="5">
+        <f t="shared" si="1"/>
         <v>-26.229199999999999</v>
       </c>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-      <c r="L49" s="6"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="1">
@@ -1464,17 +1463,17 @@
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="6">
-        <f>(A50*0.36) - 17.96</f>
+      <c r="E50" s="5">
+        <f t="shared" si="1"/>
         <v>-26.052800000000001</v>
       </c>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="1">
@@ -1483,17 +1482,17 @@
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
-      <c r="E51" s="6">
-        <f>(A51*0.36) - 17.96</f>
+      <c r="E51" s="5">
+        <f t="shared" si="1"/>
         <v>-25.174399999999999</v>
       </c>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="1">
@@ -1502,17 +1501,17 @@
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
-      <c r="E52" s="6">
-        <f>(A52*0.36) - 17.96</f>
+      <c r="E52" s="5">
+        <f t="shared" si="1"/>
         <v>-28.166</v>
       </c>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="1">
@@ -1521,17 +1520,17 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="6">
-        <f>(A53*0.36) - 17.96</f>
-        <v>-25.703600000000002</v>
-      </c>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
-      <c r="L53" s="6"/>
+      <c r="E53" s="5">
+        <f t="shared" si="1"/>
+        <v>-25.703600000000002</v>
+      </c>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>